<commit_message>
Fixed crash on blank cell in patterns file
</commit_message>
<xml_diff>
--- a/Patterns.xlsx
+++ b/Patterns.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t xml:space="preserve">UniverseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FailClose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(\d{4}-\d{2}-\d{2} \d{2}:\d{2}:\d{2},\d{3}) \[pool-(\d*?)-thread-(\d*?)].*?Failed to close document with ID : #(\d*?) http return code :  (\d*?) #$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I_httpCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NotAvail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(\d{4}-\d{2}-\d{2} \d{2}:\d{2}:\d{2},\d{3}) \[pool-(\d*?)-thread-(\d*?)].*?WebService error code: (.*?)# Http return code : (\d*?)# error message : The resource of type "(.*?)" with identifier "(\d*?)" is not available .*?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwsCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docType</t>
   </si>
 </sst>
 </file>
@@ -77,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,6 +119,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,6 +178,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -172,21 +202,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="116.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="168.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.4"/>
   </cols>
@@ -247,6 +277,59 @@
       <c r="J3" s="1" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>